<commit_message>
bump to 524, acta rename
</commit_message>
<xml_diff>
--- a/output/_abbreviation_history.xlsx
+++ b/output/_abbreviation_history.xlsx
@@ -11,6 +11,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2207271241" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2208011108" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2212061040" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2301260924" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2301260928" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3278,4 +3280,1902 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToWidth="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dept. abbr.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Inst. abbr.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Institute</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fac. abbr.</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Obsolete terms</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fgb-acesh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Academic Center for Education, Sport and Health</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>vu-alab</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>A-LAB</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>acta</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Academic Centre for Dentistry in Amsterdam</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>vu-cic</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sbe-acc</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vu-aimms</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AIMMS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fgb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Faculty of Behavioural and Movement Sciences</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>acta-fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fgw-acha</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Art and Culture, History, Antiquity</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>vu-abri</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Amsterdam Business Research Institute</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fgw</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Faculty of Humanities</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>vu-kcdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>beta-ai</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Athena Institute</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>vu-ams</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Amsterdam Movement Sciences</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>rch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Faculty of Law</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>vu-whocc</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>frt-bp</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Beliefs and Practices</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vu-an</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Amsterdam Neuroscience</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>frt</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Faculty of Religion and Theology</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>vu-acwfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>fgb-bp</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Biological Psychology</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>vu-aph</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Amsterdam Public Health</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Faculty of Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>beta-cncr</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Center for Neurogenomics and Cognitive Research</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vu-ard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Amsterdam Reproduction &amp; Development</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fsw</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Faculty of Social Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>beta-cps</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Chemistry and Pharmaceutical Sciences</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vu-asi</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Amsterdam Sustainability Institute</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sbe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>School of Business and Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>fgb-cndp</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Clinical, Neuro- &amp; Developmental Psychology</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>vu-clue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CLUE+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gnk</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VUmc - School of Medical Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>fsw-cosc</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Communication Science</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vu-ibba</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IBBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>beta-cs</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>vu-isr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Institute for Societal Resilience</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>rch-cal</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Constitutional and Administrative Law</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>vu-ki</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kooijmans Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>rch-clc</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Criminal Law and Criminology</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>vu-learn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LEARN!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rch-dpl</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Dutch Private Law</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>vu-laser</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LaserLaB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>beta-es</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Earth Sciences</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>vu-ni</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Network Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ecological Science</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>vu-tain</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Talma Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sbe-eds</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Econometrics and Data Science</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vu-ti</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tinbergen Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sbe-econ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fgb-efs</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Educational and Family Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>beta-eh</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Environment and Health</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>sbe-egs</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Ethics, Governance and Society</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>fgb-eap</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Experimental and Applied Psychology</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>sbe-fin</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>beta-hs</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Health Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>beta-hsas</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>History and Social Aspects of Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>fgb-hms</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Human Movement Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>beta-ies</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Institute for Environmental Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>beta-kggb</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>sbe-kii</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Knowledge, Information and Innovation</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>fgw-llc</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Language, Literature and Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>rch-ltlh</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Legal Theory and Legal History</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sbe-mo</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Management and Organisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>sbe-mrk</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>beta-math</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>beta-mcb</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Molecular Cell Biology</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>rch-ntl</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Notary and Tax Law</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>acta-owi</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>OWI (ACTA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>sbe-oa</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Operations Analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>acta-oii</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Oral Infections and Inflammation (OII)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>acta-orm</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Oral Regenerative Medicine (ORM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>fsw-os</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Organization Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fgw-phil</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>beta-pa</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Physics and Astronomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>fsw-pspa</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Political Science and Public Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>fsw-sca</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Social and Cultural Anthropology</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>fsw-socio</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>sbe-se</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Spatial Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>frt-tt</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Texts and Traditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>rch-tls</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Transnational Legal Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>sbe-vsee</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>VU SBE Executive Education</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup fitToWidth="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dept. abbr.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Inst. abbr.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Institute</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fac. abbr.</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Obsolete terms</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fgb-acesh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Academic Center for Education, Sport and Health</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>vu-alab</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>A-LAB</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>acta</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Academic Centre for Dentistry Amsterdam</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>acta-fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sbe-acc</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vu-aimms</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AIMMS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fgb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Faculty of Behavioural and Movement Sciences</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>vu-cic</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>beta-aile</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Amsterdam Institute for Life and Environment</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>vu-abri</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Amsterdam Business Research Institute</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fgw</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Faculty of Humanities</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fgw-acha</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Art and Culture, History, Antiquity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>vu-ams</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Amsterdam Movement Sciences</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>rch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Faculty of Law</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>vu-acwfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>beta-ai</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Athena Institute</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vu-an</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Amsterdam Neuroscience</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>frt</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Faculty of Religion and Theology</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>acta-acdia</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>frt-bp</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Beliefs and Practices</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>vu-aph</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Amsterdam Public Health</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Faculty of Science</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>vu-whocc</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fgb-bp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Biological Psychology</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vu-ard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Amsterdam Reproduction &amp; Development</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fsw</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Faculty of Social Sciences</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>vu-kcdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>beta-cncr</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Center for Neurogenomics and Cognitive Research</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vu-asi</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Amsterdam Sustainability Institute</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sbe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>School of Business and Economics</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>beta-mcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>beta-cps</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chemistry and Pharmaceutical Sciences</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>vu-clue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CLUE+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gnk</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VUmc - School of Medical Sciences</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>beta-eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>fgb-cndp</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Clinical, Neuro- &amp; Developmental Psychology</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vu-ibba</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IBBA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>fsw-cosc</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Communication Science</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>vu-isr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Institute for Societal Resilience</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>beta-cs</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>vu-ki</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kooijmans Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>rch-cal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Constitutional and Administrative Law</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>vu-learn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LEARN!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rch-clc</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Criminal Law and Criminology</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>vu-laser</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LaserLaB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rch-dpl</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Dutch Private Law</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>vu-ni</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Network Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>beta-es</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Earth Sciences</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>vu-tain</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Talma Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sbe-eds</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Econometrics and Data Science</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vu-ti</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tinbergen Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sbe-econ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fgb-efs</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Educational and Family Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>sbe-egs</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ethics, Governance and Society</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>fgb-eap</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Experimental and Applied Psychology</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>sbe-fin</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>beta-hs</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Health Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>beta-hsas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>History and Social Aspects of Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fgb-hms</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Human Movement Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>beta-ies</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Institute for Environmental Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>beta-kggb</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>sbe-kii</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Knowledge, Information and Innovation</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>fgw-llc</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Language, Literature and Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>rch-ltlh</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Legal Theory and Legal History</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>sbe-mo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Management and Organisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sbe-mrk</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>beta-math</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>rch-ntl</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Notary and Tax Law</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>acta-owi</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>OWI (ACTA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>sbe-oa</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Operations Analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>acta-oii</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Oral Infections and Inflammation (OII)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>acta-orm</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Oral Regenerative Medicine (ORM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fsw-os</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Organization Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>fgw-phil</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>beta-pa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Physics and Astronomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fsw-pspa</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Political Science and Public Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fsw-sca</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Social and Cultural Anthropology</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>fsw-socio</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>sbe-se</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Spatial Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>frt-tt</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Texts and Traditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>rch-tls</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Transnational Legal Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sbe-vsee</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>VU SBE Executive Education</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup fitToWidth="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
revert alife to aile, already used in Yoda
</commit_message>
<xml_diff>
--- a/output/_abbreviation_history.xlsx
+++ b/output/_abbreviation_history.xlsx
@@ -15,6 +15,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2301260928" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2303021440" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2303021443" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2303281656" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2303281657" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,6 +438,958 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dept. abbr.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Inst. abbr.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Institute</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fac. abbr.</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Obsolete terms</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fgb-acesh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Academic Center for Education, Sport and Health</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>vu-alab</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>A-LAB</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>acta</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Academic Centre for Dentistry Amsterdam</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>acta-fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sbe-acc</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vu-aimms</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AIMMS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fgb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Faculty of Behavioural and Movement Sciences</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>acta-acdia</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>beta-aile</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Amsterdam Institute for Life and Environment</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>vu-abri</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Amsterdam Business Research Institute</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fgw</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Faculty of Humanities</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>vu-whocc</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fgw-acha</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Art and Culture, History, Antiquity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>vu-ams</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Amsterdam Movement Sciences</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>rch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Faculty of Law</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>beta-eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>beta-ai</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Athena Institute</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vu-an</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Amsterdam Neuroscience</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>frt</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Faculty of Religion and Theology</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>beta-aminlien</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>frt-bp</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Beliefs and Practices</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>vu-aph</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Amsterdam Public Health</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Faculty of Science</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>beta-mcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fgb-bp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Biological Psychology</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vu-ard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Amsterdam Reproduction &amp; Development</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fsw</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Faculty of Social Sciences</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>beta-cncr</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Center for Neurogenomics and Cognitive Research</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vu-asi</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Amsterdam Sustainability Institute</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sbe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>School of Business and Economics</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>vu-acwfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>beta-cps</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chemistry and Pharmaceutical Sciences</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>vu-clue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CLUE+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gnk</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VUmc - School of Medical Sciences</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>vu-cic</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>fgb-cndp</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Clinical, Neuro- &amp; Developmental Psychology</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vu-ibba</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IBBA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>vu-kcdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>fsw-cosc</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Communication Science</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>vu-isr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Institute for Societal Resilience</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>beta-cs</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>vu-ki</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kooijmans Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>rch-cal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Constitutional and Administrative Law</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>vu-learn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LEARN!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rch-clc</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Criminal Law and Criminology</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>vu-laser</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LaserLaB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rch-dpl</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Dutch Private Law</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>vu-ni</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Network Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>beta-es</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Earth Sciences</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>vu-tain</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Talma Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sbe-eds</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Econometrics and Data Science</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vu-ti</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tinbergen Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sbe-econ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fgb-efs</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Educational and Family Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>sbe-egs</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ethics, Governance and Society</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>fgb-eap</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Experimental and Applied Psychology</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>sbe-fin</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>beta-hs</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Health Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>beta-hsas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>History and Social Aspects of Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fgb-hms</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Human Movement Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>beta-ies</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Institute for Environmental Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>beta-kggb</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>sbe-kii</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Knowledge, Information and Innovation</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>fgw-llc</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Language, Literature and Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>rch-ltlh</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Legal Theory and Legal History</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>sbe-mo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Management and Organisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sbe-mrk</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>beta-math</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>rch-ntl</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Notary and Tax Law</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>acta-owi</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>OWI (ACTA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>sbe-oa</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Operations Analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>acta-oii</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Oral Infections and Inflammation (OII)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>acta-orm</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Oral Regenerative Medicine (ORM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fsw-os</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Organization Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>fgw-phil</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>beta-pa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Physics and Astronomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fsw-pspa</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Political Science and Public Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fsw-sca</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Social and Cultural Anthropology</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>fsw-socio</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>sbe-se</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Spatial Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>frt-tt</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Texts and Traditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>rch-tls</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Transnational Legal Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sbe-vsee</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>VU SBE Executive Education</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup fitToWidth="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -7084,4 +8038,961 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToWidth="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dept. abbr.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Inst. abbr.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Institute</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fac. abbr.</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Obsolete terms</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fgb-acesh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Academic Center for Education, Sport and Health</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>vu-alab</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>A-LAB</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>acta</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Academic Centre for Dentistry Amsterdam</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>acta-fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sbe-acc</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vu-aimms</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AIMMS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fgb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Faculty of Behavioural and Movement Sciences</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>beta-aminlien</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Amsterdam Institute for Life and Environment</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>vu-abri</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Amsterdam Business Research Institute</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fgw</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Faculty of Humanities</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>beta-mcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fgw-acha</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Art and Culture, History, Antiquity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>vu-ams</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Amsterdam Movement Sciences</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>rch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Faculty of Law</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>vu-whocc</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>beta-ai</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Athena Institute</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vu-an</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Amsterdam Neuroscience</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>frt</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Faculty of Religion and Theology</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>beta-aile</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>frt-bp</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Beliefs and Practices</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>vu-aph</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Amsterdam Public Health</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Faculty of Science</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>beta-alife</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fgb-bp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Biological Psychology</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vu-ard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Amsterdam Reproduction &amp; Development</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fsw</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Faculty of Social Sciences</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>vu-cic</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>beta-cncr</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Center for Neurogenomics and Cognitive Research</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vu-asi</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Amsterdam Sustainability Institute</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sbe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>School of Business and Economics</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>vu-kcdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>beta-cps</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chemistry and Pharmaceutical Sciences</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>vu-clue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CLUE+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gnk</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VUmc - School of Medical Sciences</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>beta-eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>fgb-cndp</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Clinical, Neuro- &amp; Developmental Psychology</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vu-ibba</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IBBA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>vu-acwfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>fsw-cosc</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Communication Science</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>vu-isr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Institute for Societal Resilience</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>acta-acdia</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>beta-cs</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>vu-ki</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kooijmans Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>rch-cal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Constitutional and Administrative Law</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>vu-learn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LEARN!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rch-clc</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Criminal Law and Criminology</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>vu-laser</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LaserLaB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rch-dpl</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Dutch Private Law</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>vu-ni</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Network Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>beta-es</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Earth Sciences</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>vu-tain</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Talma Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sbe-eds</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Econometrics and Data Science</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vu-ti</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tinbergen Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sbe-econ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fgb-efs</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Educational and Family Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>sbe-egs</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ethics, Governance and Society</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>fgb-eap</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Experimental and Applied Psychology</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>sbe-fin</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>beta-hs</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Health Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>beta-hsas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>History and Social Aspects of Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fgb-hms</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Human Movement Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>beta-ies</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Institute for Environmental Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>beta-kggb</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>sbe-kii</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Knowledge, Information and Innovation</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>fgw-llc</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Language, Literature and Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>rch-ltlh</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Legal Theory and Legal History</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>sbe-mo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Management and Organisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sbe-mrk</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>beta-math</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>rch-ntl</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Notary and Tax Law</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>acta-owi</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>OWI (ACTA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>sbe-oa</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Operations Analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>acta-oii</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Oral Infections and Inflammation (OII)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>acta-orm</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Oral Regenerative Medicine (ORM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fsw-os</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Organization Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>fgw-phil</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>beta-pa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Physics and Astronomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fsw-pspa</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Political Science and Public Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fsw-sca</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Social and Cultural Anthropology</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>fsw-socio</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>sbe-se</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Spatial Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>frt-tt</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Texts and Traditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>rch-tls</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Transnational Legal Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sbe-vsee</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>VU SBE Executive Education</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup fitToWidth="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
list for servicenow form
</commit_message>
<xml_diff>
--- a/output/_abbreviation_history.xlsx
+++ b/output/_abbreviation_history.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18274" tabRatio="600" firstSheet="0" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,22 +18,29 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2303281657" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2305151152" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2306211159" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2307051749" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2307051751" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -60,12 +66,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -434,7 +441,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -452,7 +459,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -1388,7 +1395,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -1399,6 +1405,1908 @@
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dept. abbr.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Inst. abbr.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Institute</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fac. abbr.</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Obsolete terms</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fgb-acesh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Academic Center for Education, Sport and Health</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>vu-alab</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>A-LAB</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>acta</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Academic Centre for Dentistry Amsterdam</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>vu-whocc</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sbe-acc</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vu-aimms</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AIMMS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fgb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Faculty of Behavioural and Movement Sciences</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>vu-kcdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>beta-aile</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Amsterdam Institute for Life and Environment</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>vu-abri</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Amsterdam Business Research Institute</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fgw</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Faculty of Humanities</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>beta-aminlien</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fgw-acha</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Art and Culture, History, Antiquity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>vu-ams</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Amsterdam Movement Sciences</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>rch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Faculty of Law</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>acta-acdia</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>beta-ai</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Athena Institute</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vu-an</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Amsterdam Neuroscience</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>frt</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Faculty of Religion and Theology</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>frt-bp</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Beliefs and Practices</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>vu-aph</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Amsterdam Public Health</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Faculty of Science</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>vu-acwfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fgb-bp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Biological Psychology</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vu-ard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Amsterdam Reproduction &amp; Development</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fsw</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Faculty of Social Sciences</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>vu-cic</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>beta-cncr</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Center for Neurogenomics and Cognitive Research</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vu-asi</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Amsterdam Sustainability Institute</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sbe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>School of Business and Economics</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>acta-fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>beta-cps</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chemistry and Pharmaceutical Sciences</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>vu-clue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CLUE+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gnk</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VUmc - School of Medical Sciences</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>beta-eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>fgb-cndp</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Clinical, Neuro- &amp; Developmental Psychology</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vu-ibba</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IBBA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>beta-mcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>fsw-cosc</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Communication Science</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>vu-isr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Institute for Societal Resilience</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>beta-cs</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>vu-ki</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kooijmans Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>rch-cal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Constitutional and Administrative Law</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>vu-learn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LEARN!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rch-clc</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Criminal Law and Criminology</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>vu-laser</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LaserLaB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rch-dpl</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Dutch Private Law</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>vu-ni</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Network Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>beta-es</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Earth Sciences</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>vu-tain</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Talma Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sbe-eds</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Econometrics and Data Science</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vu-ti</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tinbergen Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sbe-econ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fgb-efs</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Educational and Family Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>sbe-egs</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ethics, Governance and Society</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>fgb-eap</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Experimental and Applied Psychology</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>sbe-fin</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>beta-hs</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Health Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>beta-hsas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>History and Social Aspects of Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fgb-hms</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Human Movement Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>beta-ies</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Institute for Environmental Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>beta-kggb</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>sbe-kii</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Knowledge, Information and Innovation</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>fgw-llc</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Language, Literature and Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>rch-ltlh</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Legal Theory and Legal History</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>sbe-mo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Management and Organisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sbe-mrk</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>beta-math</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>rch-ntl</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Notary and Tax Law</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>acta-owi</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>OWI (ACTA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>sbe-oa</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Operations Analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>acta-oii</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Oral Infections and Inflammation (OII)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>acta-orm</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Oral Regenerative Medicine (ORM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fsw-os</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Organization Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>fgw-phil</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>beta-pa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Physics and Astronomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fsw-pspa</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Political Science and Public Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fsw-sca</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Social and Cultural Anthropology</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>fsw-socio</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>sbe-se</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Spatial Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>frt-tt</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Texts and Traditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>rch-tls</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Transnational Legal Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sbe-vsee</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>VU SBE Executive Education</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dept. abbr.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Inst. abbr.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Institute</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fac. abbr.</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Obsolete terms</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fgb-acesh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Academic Center for Education, Sport and Health</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>vu-alab</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>A-LAB</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>acta</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Academic Centre for Dentistry Amsterdam</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>beta-aminlien</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sbe-acc</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vu-aimms</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AIMMS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fgb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Faculty of Behavioural and Movement Sciences</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>vu-whocc</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>beta-aile</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Amsterdam Institute for Life and Environment</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>vu-abri</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Amsterdam Business Research Institute</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fgw</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Faculty of Humanities</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>acta-fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fgw-acha</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Art and Culture, History, Antiquity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>vu-ams</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Amsterdam Movement Sciences</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>rch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Faculty of Law</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>vu-kcdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>beta-ai</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Athena Institute</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vu-an</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Amsterdam Neuroscience</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>frt</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Faculty of Religion and Theology</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>beta-eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>frt-bp</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Beliefs and Practices</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>vu-aph</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Amsterdam Public Health</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Faculty of Science</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>acta-acdia</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fgb-bp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Biological Psychology</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vu-ard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Amsterdam Reproduction &amp; Development</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fsw</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Faculty of Social Sciences</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>beta-cncr</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Center for Neurogenomics and Cognitive Research</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vu-asi</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Amsterdam Sustainability Institute</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sbe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>School of Business and Economics</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>vu-acwfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>beta-cps</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chemistry and Pharmaceutical Sciences</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>vu-clue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CLUE+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gnk</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VUmc - School of Medical Sciences</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>beta-mcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>fgb-cndp</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Clinical, Neuro- &amp; Developmental Psychology</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vu-ibba</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IBBA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>vu-cic</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>fsw-cosc</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Communication Science</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>vu-isr</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Institute for Societal Resilience</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>beta-cs</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>vu-ki</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kooijmans Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>rch-cal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Constitutional and Administrative Law</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>vu-learn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LEARN!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rch-clc</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Criminal Law and Criminology</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>vu-laser</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LaserLaB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rch-dpl</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Dutch Private Law</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>vu-ni</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Network Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>beta-es</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Earth Sciences</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>vu-tain</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Talma Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sbe-eds</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Econometrics and Data Science</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vu-ti</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tinbergen Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sbe-econ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fgb-efs</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Educational and Family Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>sbe-egs</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ethics, Governance and Society</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>fgb-eap</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Experimental and Applied Psychology</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>sbe-fin</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>beta-hs</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Health Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>beta-hsas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>History and Social Aspects of Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fgb-hms</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Human Movement Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>beta-ies</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Institute for Environmental Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>beta-kggb</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>sbe-kii</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Knowledge, Information and Innovation</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>fgw-llc</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Language, Literature and Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>rch-ltlh</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Legal Theory and Legal History</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>sbe-mo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Management and Organisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sbe-mrk</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>beta-math</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>rch-ntl</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Notary and Tax Law</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>acta-owi</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>OWI (ACTA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>sbe-oa</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Operations Analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>acta-oii</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Oral Infections and Inflammation (OII)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>acta-orm</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Oral Regenerative Medicine (ORM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fsw-os</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Organization Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>fgw-phil</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>beta-pa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Physics and Astronomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>fsw-pspa</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Political Science and Public Administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fsw-sca</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Social and Cultural Anthropology</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>fsw-socio</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>sbe-se</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Spatial Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>frt-tt</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Texts and Traditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>rch-tls</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Transnational Legal Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sbe-vsee</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>VU SBE Executive Education</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1416,37 +3324,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Dept. abbr.</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Department</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Inst. abbr.</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Institute</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Fac. abbr.</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Faculty</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Obsolete terms</t>
         </is>
@@ -1485,7 +3393,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>vu-whocc</t>
+          <t>acta-fda</t>
         </is>
       </c>
     </row>
@@ -1522,14 +3430,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>vu-kcdi</t>
+          <t>acta-acdia</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>beta-aile</t>
+          <t>beta-alife</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1559,7 +3467,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>beta-aminlien</t>
+          <t>beta-hsas</t>
         </is>
       </c>
     </row>
@@ -1596,7 +3504,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>acta-acdia</t>
+          <t>vu-acwfs</t>
         </is>
       </c>
     </row>
@@ -1633,7 +3541,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>beta-ecsc</t>
+          <t>vu-whocc</t>
         </is>
       </c>
     </row>
@@ -1670,7 +3578,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>vu-acwfs</t>
+          <t>vu-kcdi</t>
         </is>
       </c>
     </row>
@@ -1707,7 +3615,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>vu-cic</t>
+          <t>beta-aminlien</t>
         </is>
       </c>
     </row>
@@ -1744,7 +3652,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>acta-fda</t>
+          <t>beta-eh</t>
         </is>
       </c>
     </row>
@@ -1781,7 +3689,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>beta-eh</t>
+          <t>beta-mcb</t>
         </is>
       </c>
     </row>
@@ -1808,7 +3716,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>beta-mcb</t>
+          <t>vu-cic</t>
         </is>
       </c>
     </row>
@@ -1833,6 +3741,11 @@
           <t>Institute for Societal Resilience</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>beta-aile</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1855,6 +3768,11 @@
           <t>Kooijmans Institute</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2041,298 +3959,286 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>beta-hsas</t>
+          <t>fgb-hms</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>History and Social Aspects of Science</t>
+          <t>Human Movement Sciences</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>fgb-hms</t>
+          <t>beta-ies</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Human Movement Sciences</t>
+          <t>Institute for Environmental Studies</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>beta-ies</t>
+          <t>beta-kggb</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Institute for Environmental Studies</t>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>beta-kggb</t>
+          <t>sbe-kii</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Kars Group (Geo- and Bioarchaeology)</t>
+          <t>Knowledge, Information and Innovation</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>sbe-kii</t>
+          <t>fgw-llc</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Knowledge, Information and Innovation</t>
+          <t>Language, Literature and Communication</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>fgw-llc</t>
+          <t>rch-ltlh</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Language, Literature and Communication</t>
+          <t>Legal Theory and Legal History</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>rch-ltlh</t>
+          <t>sbe-mo</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Legal Theory and Legal History</t>
+          <t>Management and Organisation</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>sbe-mo</t>
+          <t>sbe-mrk</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Management and Organisation</t>
+          <t>Marketing</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>sbe-mrk</t>
+          <t>beta-math</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Mathematics</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>beta-math</t>
+          <t>rch-ntl</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Notary and Tax Law</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>rch-ntl</t>
+          <t>acta-owi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Notary and Tax Law</t>
+          <t>OWI (ACTA)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>acta-owi</t>
+          <t>sbe-oa</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>OWI (ACTA)</t>
+          <t>Operations Analytics</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>sbe-oa</t>
+          <t>acta-oii</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Operations Analytics</t>
+          <t>Oral Infections and Inflammation (OII)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>acta-oii</t>
+          <t>acta-orm</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Oral Infections and Inflammation (OII)</t>
+          <t>Oral Regenerative Medicine (ORM)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>acta-orm</t>
+          <t>fsw-os</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Oral Regenerative Medicine (ORM)</t>
+          <t>Organization Sciences</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>fsw-os</t>
+          <t>fgw-phil</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Organization Sciences</t>
+          <t>Philosophy</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>fgw-phil</t>
+          <t>beta-pa</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Philosophy</t>
+          <t>Physics and Astronomy</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>beta-pa</t>
+          <t>fsw-pspa</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Physics and Astronomy</t>
+          <t>Political Science and Public Administration</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>fsw-pspa</t>
+          <t>fsw-sca</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Political Science and Public Administration</t>
+          <t>Social and Cultural Anthropology</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>fsw-sca</t>
+          <t>fsw-socio</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Social and Cultural Anthropology</t>
+          <t>Sociology</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>fsw-socio</t>
+          <t>sbe-se</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sociology</t>
+          <t>Spatial Economics</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>sbe-se</t>
+          <t>frt-tt</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Spatial Economics</t>
+          <t>Texts and Traditions</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>frt-tt</t>
+          <t>rch-tls</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Texts and Traditions</t>
+          <t>Transnational Legal Studies</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>rch-tls</t>
+          <t>sbe-vsee</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
-        <is>
-          <t>Transnational Legal Studies</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>sbe-vsee</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
         <is>
           <t>VU SBE Executive Education</t>
         </is>
@@ -2344,13 +4250,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2368,37 +4274,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Dept. abbr.</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Department</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Inst. abbr.</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Institute</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Fac. abbr.</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Faculty</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Obsolete terms</t>
         </is>
@@ -2474,14 +4380,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>vu-whocc</t>
+          <t>beta-aile</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>beta-aile</t>
+          <t>beta-alife</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2511,7 +4417,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>acta-fda</t>
+          <t>beta-hsas</t>
         </is>
       </c>
     </row>
@@ -2548,7 +4454,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>vu-kcdi</t>
+          <t>beta-mcb</t>
         </is>
       </c>
     </row>
@@ -2585,7 +4491,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>beta-eh</t>
+          <t>vu-kcdi</t>
         </is>
       </c>
     </row>
@@ -2622,7 +4528,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>acta-acdia</t>
+          <t>vu-cic</t>
         </is>
       </c>
     </row>
@@ -2659,7 +4565,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>beta-ecsc</t>
+          <t>vu-acwfs</t>
         </is>
       </c>
     </row>
@@ -2696,7 +4602,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>vu-acwfs</t>
+          <t>beta-eh</t>
         </is>
       </c>
     </row>
@@ -2733,7 +4639,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>beta-mcb</t>
+          <t>vu-whocc</t>
         </is>
       </c>
     </row>
@@ -2760,7 +4666,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>vu-cic</t>
+          <t>acta-fda</t>
         </is>
       </c>
     </row>
@@ -2785,6 +4691,11 @@
           <t>Institute for Societal Resilience</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>acta-acdia</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2807,6 +4718,11 @@
           <t>Kooijmans Institute</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>beta-ecsc</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2993,298 +4909,286 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>beta-hsas</t>
+          <t>fgb-hms</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>History and Social Aspects of Science</t>
+          <t>Human Movement Sciences</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>fgb-hms</t>
+          <t>beta-ies</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Human Movement Sciences</t>
+          <t>Institute for Environmental Studies</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>beta-ies</t>
+          <t>beta-kggb</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Institute for Environmental Studies</t>
+          <t>Kars Group (Geo- and Bioarchaeology)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>beta-kggb</t>
+          <t>sbe-kii</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Kars Group (Geo- and Bioarchaeology)</t>
+          <t>Knowledge, Information and Innovation</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>sbe-kii</t>
+          <t>fgw-llc</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Knowledge, Information and Innovation</t>
+          <t>Language, Literature and Communication</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>fgw-llc</t>
+          <t>rch-ltlh</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Language, Literature and Communication</t>
+          <t>Legal Theory and Legal History</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>rch-ltlh</t>
+          <t>sbe-mo</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Legal Theory and Legal History</t>
+          <t>Management and Organisation</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>sbe-mo</t>
+          <t>sbe-mrk</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Management and Organisation</t>
+          <t>Marketing</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>sbe-mrk</t>
+          <t>beta-math</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Mathematics</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>beta-math</t>
+          <t>rch-ntl</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Notary and Tax Law</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>rch-ntl</t>
+          <t>acta-owi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Notary and Tax Law</t>
+          <t>OWI (ACTA)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>acta-owi</t>
+          <t>sbe-oa</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>OWI (ACTA)</t>
+          <t>Operations Analytics</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>sbe-oa</t>
+          <t>acta-oii</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Operations Analytics</t>
+          <t>Oral Infections and Inflammation (OII)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>acta-oii</t>
+          <t>acta-orm</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Oral Infections and Inflammation (OII)</t>
+          <t>Oral Regenerative Medicine (ORM)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>acta-orm</t>
+          <t>fsw-os</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Oral Regenerative Medicine (ORM)</t>
+          <t>Organization Sciences</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>fsw-os</t>
+          <t>fgw-phil</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Organization Sciences</t>
+          <t>Philosophy</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>fgw-phil</t>
+          <t>beta-pa</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Philosophy</t>
+          <t>Physics and Astronomy</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>beta-pa</t>
+          <t>fsw-pspa</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Physics and Astronomy</t>
+          <t>Political Science and Public Administration</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>fsw-pspa</t>
+          <t>fsw-sca</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Political Science and Public Administration</t>
+          <t>Social and Cultural Anthropology</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>fsw-sca</t>
+          <t>fsw-socio</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Social and Cultural Anthropology</t>
+          <t>Sociology</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>fsw-socio</t>
+          <t>sbe-se</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sociology</t>
+          <t>Spatial Economics</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>sbe-se</t>
+          <t>frt-tt</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Spatial Economics</t>
+          <t>Texts and Traditions</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>frt-tt</t>
+          <t>rch-tls</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Texts and Traditions</t>
+          <t>Transnational Legal Studies</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>rch-tls</t>
+          <t>sbe-vsee</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
-        <is>
-          <t>Transnational Legal Studies</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>sbe-vsee</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
         <is>
           <t>VU SBE Executive Education</t>
         </is>
@@ -3305,10 +5209,10 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -4248,7 +6152,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -4264,7 +6167,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -5189,7 +7092,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -5205,7 +7107,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -6140,7 +8042,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -6156,7 +8057,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -7091,7 +8992,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -7107,7 +9007,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -8038,7 +9938,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -8054,7 +9953,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -8990,7 +10889,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -9006,7 +10904,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -9942,7 +11840,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -9958,7 +11855,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="47" customWidth="1" min="2" max="2"/>
@@ -10899,6 +12796,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToWidth="1"/>
 </worksheet>
 </file>
</xml_diff>